<commit_message>
Colocado el panel de dados. Modificadores +/-10, +/-20, +/-30
</commit_message>
<xml_diff>
--- a/Notas de implementación.xlsx
+++ b/Notas de implementación.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Rol\EclipsePhase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noalc\Documents\Rol\Eclipse Phase\Ruleset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EB8865-17E4-4AD3-B6BC-BD34D4402DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ED28FE-D9E7-4D19-9D07-ECD4BF775839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{B93574B9-AB26-492B-8CCA-DDA2C02D231B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B93574B9-AB26-492B-8CCA-DDA2C02D231B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="300">
   <si>
     <t>X</t>
   </si>
@@ -972,12 +972,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1309,22 +1308,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527D745F-8723-4EB9-856D-E57F32087CFC}">
   <dimension ref="A1:G285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="5" width="34.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="34.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1332,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1364,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1372,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1380,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1388,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1412,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1420,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1428,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1436,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1444,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1460,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1468,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
@@ -1476,13 +1475,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
@@ -1492,9 +1493,11 @@
       <c r="D22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1504,9 +1507,11 @@
       <c r="D23">
         <v>30</v>
       </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1516,9 +1521,11 @@
       <c r="D24">
         <v>20</v>
       </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1528,18 +1535,22 @@
       <c r="D25" s="1">
         <v>10</v>
       </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1549,9 +1560,11 @@
       <c r="D27" s="1">
         <v>-10</v>
       </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
@@ -1561,9 +1574,11 @@
       <c r="D28">
         <v>-20</v>
       </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1573,15 +1588,17 @@
       <c r="D29">
         <v>-30</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>43</v>
       </c>
@@ -1589,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
@@ -1605,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1613,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
         <v>47</v>
       </c>
@@ -1621,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C36" s="1" t="s">
         <v>48</v>
       </c>
@@ -1629,22 +1646,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C38" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
         <v>52</v>
       </c>
@@ -1652,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C41" s="1" t="s">
         <v>53</v>
       </c>
@@ -1660,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C42" s="1" t="s">
         <v>54</v>
       </c>
@@ -1668,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C43" s="1" t="s">
         <v>55</v>
       </c>
@@ -1676,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C44" s="1" t="s">
         <v>56</v>
       </c>
@@ -1684,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>57</v>
       </c>
@@ -1692,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C46" s="1" t="s">
         <v>58</v>
       </c>
@@ -1700,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C47" s="1" t="s">
         <v>59</v>
       </c>
@@ -1708,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
         <v>60</v>
       </c>
@@ -1716,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C49" s="1" t="s">
         <v>61</v>
       </c>
@@ -1724,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C50" s="1" t="s">
         <v>62</v>
       </c>
@@ -1732,49 +1749,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C51" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>64</v>
       </c>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C53" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C54" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C56" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D57" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D58" s="1" t="s">
         <v>70</v>
       </c>
@@ -1782,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D59" s="1" t="s">
         <v>71</v>
       </c>
@@ -1790,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D60" s="1" t="s">
         <v>72</v>
       </c>
@@ -1798,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D61" s="1" t="s">
         <v>73</v>
       </c>
@@ -1806,19 +1823,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="D62" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1" t="s">
         <v>75</v>
       </c>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D64" s="1" t="s">
         <v>76</v>
       </c>
@@ -1826,13 +1843,13 @@
         <v>299</v>
       </c>
     </row>
-    <row r="65" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D65" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D66" s="1" t="s">
         <v>78</v>
       </c>
@@ -1840,17 +1857,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D68" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="3:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="D69" s="1" t="s">
         <v>81</v>
       </c>
@@ -1858,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D70" s="1" t="s">
         <v>82</v>
       </c>
@@ -1866,22 +1883,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D71" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D72" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D74" s="1" t="s">
         <v>76</v>
       </c>
@@ -1889,22 +1906,22 @@
         <v>299</v>
       </c>
     </row>
-    <row r="75" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D75" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D76" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="D78" s="1" t="s">
         <v>88</v>
       </c>
@@ -1912,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="D79" s="1" t="s">
         <v>89</v>
       </c>
@@ -1920,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="D80" s="1" t="s">
         <v>90</v>
       </c>
@@ -1928,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D81" s="1" t="s">
         <v>91</v>
       </c>
@@ -1936,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -1944,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
         <v>92</v>
       </c>
@@ -1952,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B84" s="1" t="s">
         <v>93</v>
       </c>
@@ -1960,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C85" s="1" t="s">
         <v>94</v>
       </c>
@@ -1968,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C86" s="1" t="s">
         <v>95</v>
       </c>
@@ -1976,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C87" s="1" t="s">
         <v>96</v>
       </c>
@@ -1984,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C88" s="1" t="s">
         <v>97</v>
       </c>
@@ -1992,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C89" s="1" t="s">
         <v>98</v>
       </c>
@@ -2000,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C90" s="1" t="s">
         <v>99</v>
       </c>
@@ -2008,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C91" s="1" t="s">
         <v>100</v>
       </c>
@@ -2016,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C92" s="1" t="s">
         <v>101</v>
       </c>
@@ -2024,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C93" s="1" t="s">
         <v>102</v>
       </c>
@@ -2032,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C94" s="1" t="s">
         <v>103</v>
       </c>
@@ -2040,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D95" s="1" t="s">
         <v>104</v>
       </c>
@@ -2048,12 +2065,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D96" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D97" s="1" t="s">
         <v>106</v>
       </c>
@@ -2061,12 +2078,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E98" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B99" s="1" t="s">
         <v>108</v>
       </c>
@@ -2074,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C100" s="1" t="s">
         <v>109</v>
       </c>
@@ -2082,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C101" s="1" t="s">
         <v>110</v>
       </c>
@@ -2090,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C102" s="1" t="s">
         <v>111</v>
       </c>
@@ -2098,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C103" s="1" t="s">
         <v>112</v>
       </c>
@@ -2106,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C104" s="1" t="s">
         <v>113</v>
       </c>
@@ -2114,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C105" s="1" t="s">
         <v>114</v>
       </c>
@@ -2122,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D106" s="1" t="s">
         <v>115</v>
       </c>
@@ -2130,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D107" s="1" t="s">
         <v>116</v>
       </c>
@@ -2138,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D108" s="1" t="s">
         <v>117</v>
       </c>
@@ -2146,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B109" s="1" t="s">
         <v>118</v>
       </c>
@@ -2154,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C110" s="1" t="s">
         <v>119</v>
       </c>
@@ -2162,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D111" s="1" t="s">
         <v>120</v>
       </c>
@@ -2170,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C112" s="1" t="s">
         <v>121</v>
       </c>
@@ -2178,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C113" s="1" t="s">
         <v>122</v>
       </c>
@@ -2186,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C114" s="1" t="s">
         <v>123</v>
       </c>
@@ -2194,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C115" s="1" t="s">
         <v>124</v>
       </c>
@@ -2202,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C116" s="1" t="s">
         <v>125</v>
       </c>
@@ -2210,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C117" s="1" t="s">
         <v>126</v>
       </c>
@@ -2218,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C118" s="1" t="s">
         <v>127</v>
       </c>
@@ -2226,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B119" s="1" t="s">
         <v>128</v>
       </c>
@@ -2234,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C120" s="1" t="s">
         <v>129</v>
       </c>
@@ -2242,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C121" s="1" t="s">
         <v>130</v>
       </c>
@@ -2250,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C122" s="1" t="s">
         <v>131</v>
       </c>
@@ -2258,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C123" s="1" t="s">
         <v>132</v>
       </c>
@@ -2266,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C124" s="1" t="s">
         <v>133</v>
       </c>
@@ -2274,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C125" s="1" t="s">
         <v>134</v>
       </c>
@@ -2282,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C126" s="1" t="s">
         <v>135</v>
       </c>
@@ -2290,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C127" s="1" t="s">
         <v>136</v>
       </c>
@@ -2298,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C128" s="1" t="s">
         <v>137</v>
       </c>
@@ -2306,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B129" s="1" t="s">
         <v>138</v>
       </c>
@@ -2314,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C130" s="1" t="s">
         <v>139</v>
       </c>
@@ -2322,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C131" s="1" t="s">
         <v>140</v>
       </c>
@@ -2330,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D132" s="1" t="s">
         <v>141</v>
       </c>
@@ -2338,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B133" s="1" t="s">
         <v>142</v>
       </c>
@@ -2346,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C134" s="1" t="s">
         <v>143</v>
       </c>
@@ -2354,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D135" s="1" t="s">
         <v>144</v>
       </c>
@@ -2362,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D136" s="1" t="s">
         <v>145</v>
       </c>
@@ -2370,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C137" s="1" t="s">
         <v>146</v>
       </c>
@@ -2378,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C138" s="1" t="s">
         <v>147</v>
       </c>
@@ -2386,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C139" s="1" t="s">
         <v>148</v>
       </c>
@@ -2394,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C140" s="1" t="s">
         <v>149</v>
       </c>
@@ -2402,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C141" s="1" t="s">
         <v>150</v>
       </c>
@@ -2410,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C142" s="1" t="s">
         <v>151</v>
       </c>
@@ -2418,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C143" s="1" t="s">
         <v>152</v>
       </c>
@@ -2426,17 +2443,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B144" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C145" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C146" s="1" t="s">
         <v>155</v>
       </c>
@@ -2444,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D147" s="1" t="s">
         <v>156</v>
       </c>
@@ -2452,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.35">
       <c r="E148" s="1" t="s">
         <v>157</v>
       </c>
@@ -2460,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.35">
       <c r="E149" s="1" t="s">
         <v>158</v>
       </c>
@@ -2468,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.35">
       <c r="E150" s="1" t="s">
         <v>159</v>
       </c>
@@ -2476,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D151" s="1" t="s">
         <v>160</v>
       </c>
@@ -2484,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D152" s="1" t="s">
         <v>161</v>
       </c>
@@ -2492,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C153" s="1" t="s">
         <v>162</v>
       </c>
@@ -2500,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B154" s="1" t="s">
         <v>102</v>
       </c>
@@ -2508,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B155" s="1" t="s">
         <v>96</v>
       </c>
@@ -2516,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C156" s="1" t="s">
         <v>163</v>
       </c>
@@ -2524,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D157" s="1" t="s">
         <v>164</v>
       </c>
@@ -2532,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C158" s="1" t="s">
         <v>165</v>
       </c>
@@ -2540,7 +2557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D159" s="1" t="s">
         <v>166</v>
       </c>
@@ -2548,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D160" s="1" t="s">
         <v>167</v>
       </c>
@@ -2556,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D161" s="1" t="s">
         <v>168</v>
       </c>
@@ -2564,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D162" s="1" t="s">
         <v>169</v>
       </c>
@@ -2572,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D163" s="1" t="s">
         <v>170</v>
       </c>
@@ -2580,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D164" s="1" t="s">
         <v>171</v>
       </c>
@@ -2588,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D165" s="1" t="s">
         <v>172</v>
       </c>
@@ -2596,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E166" s="1" t="s">
         <v>173</v>
       </c>
@@ -2604,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E167" s="1" t="s">
         <v>174</v>
       </c>
@@ -2612,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C168" s="1" t="s">
         <v>175</v>
       </c>
@@ -2620,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D169" s="1" t="s">
         <v>176</v>
       </c>
@@ -2628,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E170" s="1" t="s">
         <v>177</v>
       </c>
@@ -2636,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E171" s="1" t="s">
         <v>178</v>
       </c>
@@ -2644,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E172" s="1" t="s">
         <v>179</v>
       </c>
@@ -2652,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E173" s="1" t="s">
         <v>180</v>
       </c>
@@ -2660,7 +2677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>20</v>
       </c>
@@ -2671,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E175" s="1" t="s">
         <v>182</v>
       </c>
@@ -2679,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D176" s="1" t="s">
         <v>172</v>
       </c>
@@ -2687,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B177" s="1" t="s">
         <v>183</v>
       </c>
@@ -2695,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C178" s="1" t="s">
         <v>184</v>
       </c>
@@ -2703,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C179" s="1" t="s">
         <v>185</v>
       </c>
@@ -2711,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C180" s="1" t="s">
         <v>186</v>
       </c>
@@ -2719,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C181" s="1" t="s">
         <v>187</v>
       </c>
@@ -2727,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B182" s="1" t="s">
         <v>188</v>
       </c>
@@ -2735,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C183" s="1" t="s">
         <v>189</v>
       </c>
@@ -2743,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C184" s="1" t="s">
         <v>190</v>
       </c>
@@ -2751,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C185" s="1" t="s">
         <v>191</v>
       </c>
@@ -2759,12 +2776,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B187" s="1" t="s">
         <v>193</v>
       </c>
@@ -2772,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C188" s="1" t="s">
         <v>194</v>
       </c>
@@ -2780,7 +2797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C189" s="1" t="s">
         <v>195</v>
       </c>
@@ -2788,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C190" s="1" t="s">
         <v>196</v>
       </c>
@@ -2796,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C191" s="1" t="s">
         <v>197</v>
       </c>
@@ -2804,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C192" s="1" t="s">
         <v>198</v>
       </c>
@@ -2812,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C193" s="1" t="s">
         <v>199</v>
       </c>
@@ -2820,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B194" s="1" t="s">
         <v>200</v>
       </c>
@@ -2828,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C195" s="1" t="s">
         <v>201</v>
       </c>
@@ -2836,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C196" s="1" t="s">
         <v>202</v>
       </c>
@@ -2844,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C197" s="1" t="s">
         <v>203</v>
       </c>
@@ -2852,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C198" s="1" t="s">
         <v>204</v>
       </c>
@@ -2860,7 +2877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C199" s="1" t="s">
         <v>205</v>
       </c>
@@ -2868,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B200" s="1" t="s">
         <v>206</v>
       </c>
@@ -2876,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C201" s="1" t="s">
         <v>207</v>
       </c>
@@ -2884,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C202" s="1" t="s">
         <v>208</v>
       </c>
@@ -2892,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C203" s="1" t="s">
         <v>209</v>
       </c>
@@ -2900,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D204" s="1" t="s">
         <v>210</v>
       </c>
@@ -2908,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C205" s="1" t="s">
         <v>211</v>
       </c>
@@ -2916,12 +2933,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B206" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="207" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C207" s="1" t="s">
         <v>213</v>
       </c>
@@ -2929,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D208" s="1" t="s">
         <v>214</v>
       </c>
@@ -2937,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C209" s="1" t="s">
         <v>215</v>
       </c>
@@ -2945,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C210" s="1" t="s">
         <v>216</v>
       </c>
@@ -2953,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C211" s="1" t="s">
         <v>217</v>
       </c>
@@ -2961,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C212" s="1" t="s">
         <v>218</v>
       </c>
@@ -2969,12 +2986,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C213" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D214" s="1" t="s">
         <v>220</v>
       </c>
@@ -2982,7 +2999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D215" s="1" t="s">
         <v>221</v>
       </c>
@@ -2990,12 +3007,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="E216" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D217" s="1" t="s">
         <v>223</v>
       </c>
@@ -3003,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D218" s="1" t="s">
         <v>224</v>
       </c>
@@ -3011,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E219" s="1" t="s">
         <v>225</v>
       </c>
@@ -3019,62 +3036,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E220" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B222" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C223" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C224" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="D225" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B226" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C227" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C228" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B231" s="1" t="s">
         <v>237</v>
       </c>
@@ -3082,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C232" s="1" t="s">
         <v>238</v>
       </c>
@@ -3090,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C233" s="1" t="s">
         <v>239</v>
       </c>
@@ -3098,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C234" s="1" t="s">
         <v>240</v>
       </c>
@@ -3106,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B235" s="1" t="s">
         <v>241</v>
       </c>
@@ -3114,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C236" s="1" t="s">
         <v>242</v>
       </c>
@@ -3122,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C237" s="1" t="s">
         <v>243</v>
       </c>
@@ -3130,7 +3147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C238" s="1" t="s">
         <v>244</v>
       </c>
@@ -3138,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C239" s="1" t="s">
         <v>245</v>
       </c>
@@ -3146,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B240" s="1" t="s">
         <v>246</v>
       </c>
@@ -3154,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C241" s="1" t="s">
         <v>247</v>
       </c>
@@ -3162,7 +3179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C242" s="1" t="s">
         <v>248</v>
       </c>
@@ -3170,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C243" s="1" t="s">
         <v>249</v>
       </c>
@@ -3178,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="D244" s="1" t="s">
         <v>250</v>
       </c>
@@ -3186,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D245" s="1" t="s">
         <v>251</v>
       </c>
@@ -3194,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D246" s="1" t="s">
         <v>252</v>
       </c>
@@ -3202,47 +3219,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B247" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="248" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C248" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B249" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="250" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C250" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="251" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C251" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="252" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C252" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="253" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:7" ht="116" x14ac:dyDescent="0.35">
       <c r="C253" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B254" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="255" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C255" s="1" t="s">
         <v>261</v>
       </c>
@@ -3250,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D256" s="1" t="s">
         <v>262</v>
       </c>
@@ -3258,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D257" s="1" t="s">
         <v>263</v>
       </c>
@@ -3266,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E258" s="1" t="s">
         <v>264</v>
       </c>
@@ -3274,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E259" s="1" t="s">
         <v>265</v>
       </c>
@@ -3282,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E260" s="1" t="s">
         <v>266</v>
       </c>
@@ -3290,7 +3307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E261" s="1" t="s">
         <v>267</v>
       </c>
@@ -3298,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E262" s="1" t="s">
         <v>268</v>
       </c>
@@ -3306,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E263" s="1" t="s">
         <v>269</v>
       </c>
@@ -3314,17 +3331,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F264" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="265" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F265" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="266" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C266" s="1" t="s">
         <v>272</v>
       </c>
@@ -3332,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D267" s="1" t="s">
         <v>273</v>
       </c>
@@ -3340,92 +3357,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C268" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="269" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D269" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="270" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D270" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="271" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E271" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="272" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E272" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="273" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:5" ht="29" x14ac:dyDescent="0.35">
       <c r="E273" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="274" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:5" ht="29" x14ac:dyDescent="0.35">
       <c r="E274" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="275" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E275" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="276" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:5" ht="29" x14ac:dyDescent="0.35">
       <c r="E276" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="277" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="D277" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="278" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C278" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="279" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D279" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="280" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:5" ht="58" x14ac:dyDescent="0.35">
       <c r="D280" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="281" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C281" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="282" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D282" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="283" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D283" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="284" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:5" ht="29" x14ac:dyDescent="0.35">
       <c r="D284" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="285" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:5" ht="58" x14ac:dyDescent="0.35">
       <c r="D285" s="1" t="s">
         <v>291</v>
       </c>
@@ -3449,40 +3466,40 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>298</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wounds y Traumas afectan a los checks e iniciativas
</commit_message>
<xml_diff>
--- a/Notas de implementación.xlsx
+++ b/Notas de implementación.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noalc\Documents\Rol\Eclipse Phase\Ruleset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ED28FE-D9E7-4D19-9D07-ECD4BF775839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFE6E9A-0AD5-4636-ADD6-494107A92856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B93574B9-AB26-492B-8CCA-DDA2C02D231B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="300">
   <si>
     <t>X</t>
   </si>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527D745F-8723-4EB9-856D-E57F32087CFC}">
   <dimension ref="A1:G285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="G223" sqref="G223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1847,7 +1847,9 @@
       <c r="D65" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G65" s="1"/>
+      <c r="G65" s="1" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="66" spans="3:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D66" s="1" t="s">
@@ -1910,6 +1912,9 @@
       <c r="D75" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="G75" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="76" spans="3:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D76" s="1" t="s">
@@ -3040,6 +3045,9 @@
       <c r="E220" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="G220" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
@@ -3079,6 +3087,9 @@
     <row r="228" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C228" s="1" t="s">
         <v>234</v>
+      </c>
+      <c r="G228" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Orden correcto al abrir el CT con actores con INI 0 y Extra Actions no puede targetearse
</commit_message>
<xml_diff>
--- a/Notas de implementación.xlsx
+++ b/Notas de implementación.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noalc\Documents\Rol\Eclipse Phase\Ruleset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFE6E9A-0AD5-4636-ADD6-494107A92856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE68DA6-414A-4BAE-899A-FBA89A001942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B93574B9-AB26-492B-8CCA-DDA2C02D231B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="300">
   <si>
     <t>X</t>
   </si>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527D745F-8723-4EB9-856D-E57F32087CFC}">
   <dimension ref="A1:G285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="G223" sqref="G223"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1596,7 +1596,9 @@
       <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
@@ -1650,10 +1652,16 @@
       <c r="B37" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="G37" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C38" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>